<commit_message>
addd graph for resnet 101 10gbps in rack, even, no striping
</commit_message>
<xml_diff>
--- a/distributed-tensorflow-simulator/exp_results/resnet-101/graphs/10gbps_inrack_even_nostriping.xlsx
+++ b/distributed-tensorflow-simulator/exp_results/resnet-101/graphs/10gbps_inrack_even_nostriping.xlsx
@@ -14,9 +14,6 @@
   <sheets>
     <sheet name="out" sheetId="1" r:id="rId1"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId2"/>
-  </externalReferences>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -261,19 +258,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>4.0259</c:v>
+                    <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>6.7364</c:v>
+                    <c:v>17.8604</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>3.0035</c:v>
+                    <c:v>8.0541</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0.9301</c:v>
+                    <c:v>11.3103</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>1.8855</c:v>
+                    <c:v>4.9555</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -285,19 +282,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>3.925</c:v>
+                    <c:v>7.5114</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>10.4181</c:v>
+                    <c:v>0.8628</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>12.7606</c:v>
+                    <c:v>1.2145</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>8.9398</c:v>
+                    <c:v>9.5644</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>3.5476</c:v>
+                    <c:v>4.4925</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -350,16 +347,16 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0</c:v>
+                  <c:v>-4.2132</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.5097</c:v>
+                  <c:v>1.7411</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.2364</c:v>
+                  <c:v>2.5525</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.3164</c:v>
+                  <c:v>0.1073</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -408,19 +405,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>4.1947</c:v>
+                    <c:v>4.3743</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>14.985</c:v>
+                    <c:v>10.8072</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>3.7104</c:v>
+                    <c:v>4.2349</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>1.7636</c:v>
+                    <c:v>9.5878</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>5.4841</c:v>
+                    <c:v>6.0744</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -432,19 +429,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>4.2955</c:v>
+                    <c:v>2.1156</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>17.94</c:v>
+                    <c:v>12.2658</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>2.6738</c:v>
+                    <c:v>11.7957</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>6.3948</c:v>
+                    <c:v>7.2825</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>10.0563</c:v>
+                    <c:v>6.2653</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -494,19 +491,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>-4.1947</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>14.7575</c:v>
+                  <c:v>11.5968</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8.129200000000001</c:v>
+                  <c:v>6.9655</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>17.0096</c:v>
+                  <c:v>11.9672</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -555,19 +552,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.0</c:v>
+                    <c:v>1.4381</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>2.0037</c:v>
+                    <c:v>2.627</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>4.6401</c:v>
+                    <c:v>2.9829</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>30.5648</c:v>
+                    <c:v>19.3898</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>3.3438</c:v>
+                    <c:v>6.7451</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -579,19 +576,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.0</c:v>
+                    <c:v>1.9399</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>15.151</c:v>
+                    <c:v>6.1347</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>9.1227</c:v>
+                    <c:v>5.2955</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>15.9202</c:v>
+                    <c:v>22.5117</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.9725</c:v>
+                    <c:v>2.953</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -641,19 +638,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>0.8984</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0</c:v>
+                  <c:v>2.33</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9.5719</c:v>
+                  <c:v>9.4778</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-2.4572</c:v>
+                  <c:v>2.3947</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>12.7744</c:v>
+                  <c:v>10.9771</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -702,19 +699,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.0</c:v>
+                    <c:v>1.0544</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.5409</c:v>
+                    <c:v>0.6724</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>3.9909</c:v>
+                    <c:v>2.5839</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>25.4029</c:v>
+                    <c:v>13.1446</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>2.2231</c:v>
+                    <c:v>5.5522</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -726,19 +723,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.0</c:v>
+                    <c:v>0.5229</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>2.5549</c:v>
+                    <c:v>1.9568</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>24.307</c:v>
+                    <c:v>4.7347</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>52.1455</c:v>
+                    <c:v>32.7062</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>7.9821</c:v>
+                    <c:v>12.5223</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -791,16 +788,16 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0</c:v>
+                  <c:v>0.6627</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>11.1613</c:v>
+                  <c:v>6.9943</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.4196</c:v>
+                  <c:v>-0.3852</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -815,11 +812,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2090814656"/>
-        <c:axId val="-2089125648"/>
+        <c:axId val="-2093403504"/>
+        <c:axId val="-2093395472"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2090814656"/>
+        <c:axId val="-2093403504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -936,12 +933,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2089125648"/>
+        <c:crossAx val="-2093395472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2089125648"/>
+        <c:axId val="-2093395472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1071,7 +1068,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2090814656"/>
+        <c:crossAx val="-2093403504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1293,19 +1290,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>3.7273</c:v>
+                    <c:v>1.6604</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>5.1142</c:v>
+                    <c:v>14.8104</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.7876</c:v>
+                    <c:v>7.3989</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>1.3626</c:v>
+                    <c:v>12.3897</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>4.4124</c:v>
+                    <c:v>6.1835</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1317,19 +1314,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.1977</c:v>
+                    <c:v>9.8666</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.0121</c:v>
+                    <c:v>0.8288</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.0071</c:v>
+                    <c:v>1.8716</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>1.0134</c:v>
+                    <c:v>0.9607</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>1.3399</c:v>
+                    <c:v>1.9304</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1379,19 +1376,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>-3.7273</c:v>
+                  <c:v>14.1384</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-3.8555</c:v>
+                  <c:v>6.1501</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-2.2559</c:v>
+                  <c:v>2.9178</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-0.3849</c:v>
+                  <c:v>4.1162</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-0.1219</c:v>
+                  <c:v>3.3427</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1440,19 +1437,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>4.758</c:v>
+                    <c:v>5.4872</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>5.0196</c:v>
+                    <c:v>0.2378</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>5.4643</c:v>
+                    <c:v>4.6916</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>3.8494</c:v>
+                    <c:v>4.1142</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>3.3326</c:v>
+                    <c:v>3.7087</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1464,19 +1461,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>3.7322</c:v>
+                    <c:v>2.1198</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>6.7954</c:v>
+                    <c:v>9.6946</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>4.1632</c:v>
+                    <c:v>5.0204</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>1.742</c:v>
+                    <c:v>3.8872</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>1.5539</c:v>
+                    <c:v>2.6673</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1526,19 +1523,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>-4.758</c:v>
+                  <c:v>2.1198</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-5.0196</c:v>
+                  <c:v>19.4444</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.567</c:v>
+                  <c:v>18.0074</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.791</c:v>
+                  <c:v>20.5471</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>14.6713</c:v>
+                  <c:v>19.2965</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1587,19 +1584,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.0</c:v>
+                    <c:v>1.8287</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.0</c:v>
+                    <c:v>2.1029</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>19.1607</c:v>
+                    <c:v>4.869</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>10.2113</c:v>
+                    <c:v>4.7591</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>2.4683</c:v>
+                    <c:v>2.188</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1611,19 +1608,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.0</c:v>
+                    <c:v>0.105</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>25.2157</c:v>
+                    <c:v>4.7906</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>5.3919</c:v>
+                    <c:v>4.5001</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>3.9989</c:v>
+                    <c:v>6.1161</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>2.1896</c:v>
+                    <c:v>2.3285</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1673,19 +1670,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>2.1198</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0</c:v>
+                  <c:v>8.7389</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-14.0026</c:v>
+                  <c:v>18.0377</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.6069</c:v>
+                  <c:v>28.9066</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>19.3497</c:v>
+                  <c:v>28.3504</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1734,19 +1731,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.0</c:v>
+                    <c:v>0.6439</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.5409</c:v>
+                    <c:v>0.523</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>1.1014</c:v>
+                    <c:v>8.3348</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>16.4925</c:v>
+                    <c:v>18.184</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>4.0586</c:v>
+                    <c:v>1.642</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1758,19 +1755,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.0</c:v>
+                    <c:v>0.9507</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.0</c:v>
+                    <c:v>0.6764</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>23.7074</c:v>
+                    <c:v>3.171</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>72.5341</c:v>
+                    <c:v>26.9225</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>9.6737</c:v>
+                    <c:v>5.0508</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1820,19 +1817,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>2.5194</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0</c:v>
+                  <c:v>4.6391</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.4843</c:v>
+                  <c:v>7.8101</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.8021</c:v>
+                  <c:v>17.9753</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>19.6316</c:v>
+                  <c:v>33.5532</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1847,11 +1844,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2086261648"/>
-        <c:axId val="-2089788544"/>
+        <c:axId val="-2078471696"/>
+        <c:axId val="-2078465440"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2086261648"/>
+        <c:axId val="-2078471696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1968,12 +1965,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2089788544"/>
+        <c:crossAx val="-2078465440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2089788544"/>
+        <c:axId val="-2078465440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2103,7 +2100,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2086261648"/>
+        <c:crossAx val="-2078471696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2247,7 +2244,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2325,19 +2321,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>3.7273</c:v>
+                    <c:v>1.6604</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>3.9764</c:v>
+                    <c:v>12.265</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>5.672</c:v>
+                    <c:v>3.7346</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>9.4621</c:v>
+                    <c:v>6.4366</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>2.3216</c:v>
+                    <c:v>1.6465</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -2349,19 +2345,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.1977</c:v>
+                    <c:v>9.8666</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>1.152</c:v>
+                    <c:v>0.8386</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>8.9293</c:v>
+                    <c:v>9.8327</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>1.7972</c:v>
+                    <c:v>4.3782</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>1.1005</c:v>
+                    <c:v>1.7384</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -2411,19 +2407,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>-3.7273</c:v>
+                  <c:v>14.1384</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>19.4309</c:v>
+                  <c:v>27.1764</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>60.0573</c:v>
+                  <c:v>64.9414</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>65.6399</c:v>
+                  <c:v>71.6921</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>82.009</c:v>
+                  <c:v>82.6162</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2472,19 +2468,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>4.758</c:v>
+                    <c:v>5.4872</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>5.0196</c:v>
+                    <c:v>0.2378</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>11.739</c:v>
+                    <c:v>5.5377</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>7.7245</c:v>
+                    <c:v>8.3107</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>4.639</c:v>
+                    <c:v>2.6516</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -2496,19 +2492,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>3.7322</c:v>
+                    <c:v>2.1198</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>6.7954</c:v>
+                    <c:v>9.6946</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>8.2575</c:v>
+                    <c:v>9.8546</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>7.4079</c:v>
+                    <c:v>5.3022</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>1.0665</c:v>
+                    <c:v>1.6975</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -2558,19 +2554,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>-4.758</c:v>
+                  <c:v>2.1198</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-5.0196</c:v>
+                  <c:v>19.4444</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>34.7364</c:v>
+                  <c:v>50.0047</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>47.8063</c:v>
+                  <c:v>54.7683</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>71.8039</c:v>
+                  <c:v>73.4421</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2619,19 +2615,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.0</c:v>
+                    <c:v>1.8287</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.0</c:v>
+                    <c:v>2.1029</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>9.2979</c:v>
+                    <c:v>12.4279</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>18.0662</c:v>
+                    <c:v>4.5978</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>11.6696</c:v>
+                    <c:v>9.2365</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -2643,19 +2639,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.0</c:v>
+                    <c:v>0.105</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>25.2157</c:v>
+                    <c:v>4.7906</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>6.9939</c:v>
+                    <c:v>3.6305</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>7.6986</c:v>
+                    <c:v>3.8286</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>6.8492</c:v>
+                    <c:v>7.9172</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -2705,19 +2701,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>2.1198</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0</c:v>
+                  <c:v>8.7389</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.7227</c:v>
+                  <c:v>24.0578</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7.9357</c:v>
+                  <c:v>29.0445</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>50.1355</c:v>
+                  <c:v>56.5915</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2766,19 +2762,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.0</c:v>
+                    <c:v>0.6439</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.5409</c:v>
+                    <c:v>0.523</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>1.1014</c:v>
+                    <c:v>8.3348</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>16.0689</c:v>
+                    <c:v>8.0742</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>5.146</c:v>
+                    <c:v>5.3498</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -2790,19 +2786,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.0</c:v>
+                    <c:v>0.9507</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.0</c:v>
+                    <c:v>0.6764</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>23.7074</c:v>
+                    <c:v>3.171</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>69.2573</c:v>
+                    <c:v>39.0229</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>8.6863</c:v>
+                    <c:v>7.8408</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -2852,19 +2848,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>2.5194</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0</c:v>
+                  <c:v>4.6391</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.4843</c:v>
+                  <c:v>7.8101</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.3387</c:v>
+                  <c:v>14.9391</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16.4809</c:v>
+                  <c:v>31.3813</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2879,11 +2875,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2086554032"/>
-        <c:axId val="-2093741744"/>
+        <c:axId val="-2078406832"/>
+        <c:axId val="-2078400576"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2086554032"/>
+        <c:axId val="-2078406832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2933,7 +2929,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3000,12 +2995,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2093741744"/>
+        <c:crossAx val="-2078400576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2093741744"/>
+        <c:axId val="-2078400576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3068,7 +3063,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3135,7 +3129,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2086554032"/>
+        <c:crossAx val="-2078406832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3279,7 +3273,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3360,16 +3353,16 @@
                     <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.3355</c:v>
+                    <c:v>0.3499</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>5.2868</c:v>
+                    <c:v>5.8325</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>9.7923</c:v>
+                    <c:v>4.1815</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>2.0956</c:v>
+                    <c:v>2.0725</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -3384,16 +3377,16 @@
                     <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.7827</c:v>
+                    <c:v>1.1405</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>8.729</c:v>
+                    <c:v>8.9604</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>1.2827</c:v>
+                    <c:v>3.6105</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.9281</c:v>
+                    <c:v>2.9475</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -3446,16 +3439,16 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>22.0955</c:v>
+                  <c:v>23.041</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>60.9385</c:v>
+                  <c:v>62.5123</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>65.624</c:v>
+                  <c:v>69.8593</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>81.9122</c:v>
+                  <c:v>81.8118</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3510,13 +3503,13 @@
                     <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>9.1683</c:v>
+                    <c:v>9.6853</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>10.4673</c:v>
+                    <c:v>10.7974</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>5.5595</c:v>
+                    <c:v>3.0792</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -3534,13 +3527,13 @@
                     <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>15.2419</c:v>
+                    <c:v>15.7901</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>4.7426</c:v>
+                    <c:v>5.2158</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>2.1894</c:v>
+                    <c:v>2.0658</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -3596,13 +3589,13 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>37.0019</c:v>
+                  <c:v>38.4723</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>41.8236</c:v>
+                  <c:v>42.7335</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>66.9365</c:v>
+                  <c:v>67.2985</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3657,13 +3650,13 @@
                     <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>13.3538</c:v>
+                    <c:v>14.3345</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>9.4555</c:v>
+                    <c:v>5.3122</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>13.0712</c:v>
+                    <c:v>13.2272</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -3681,13 +3674,13 @@
                     <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>7.7187</c:v>
+                    <c:v>8.1956</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>4.4303</c:v>
+                    <c:v>0.891</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>9.0564</c:v>
+                    <c:v>10.3355</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -3743,13 +3736,13 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.7187</c:v>
+                  <c:v>8.1956</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.585</c:v>
+                  <c:v>-0.1156</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>38.2896</c:v>
+                  <c:v>39.0999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3807,10 +3800,10 @@
                     <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>19.9679</c:v>
+                    <c:v>20.0357</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>4.8809</c:v>
+                    <c:v>12.3859</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -3831,10 +3824,10 @@
                     <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>13.3517</c:v>
+                    <c:v>16.7757</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>12.7332</c:v>
+                    <c:v>15.6097</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -3893,10 +3886,10 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.5636</c:v>
+                  <c:v>-13.8936</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-2.7039</c:v>
+                  <c:v>-1.4443</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3911,11 +3904,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2086385824"/>
-        <c:axId val="-2086383984"/>
+        <c:axId val="-2075341424"/>
+        <c:axId val="-2075335168"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2086385824"/>
+        <c:axId val="-2075341424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3965,7 +3958,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -4032,12 +4024,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2086383984"/>
+        <c:crossAx val="-2075335168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2086383984"/>
+        <c:axId val="-2075335168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4100,7 +4092,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -4167,7 +4158,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2086385824"/>
+        <c:crossAx val="-2075341424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6609,915 +6600,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="out"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="4">
-          <cell r="D4">
-            <v>2</v>
-          </cell>
-          <cell r="E4">
-            <v>0</v>
-          </cell>
-          <cell r="F4">
-            <v>0</v>
-          </cell>
-          <cell r="G4">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="D5">
-            <v>4</v>
-          </cell>
-          <cell r="E5">
-            <v>17.238099999999999</v>
-          </cell>
-          <cell r="F5">
-            <v>0.85809999999999997</v>
-          </cell>
-          <cell r="G5">
-            <v>0.26169999999999999</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="D6">
-            <v>8</v>
-          </cell>
-          <cell r="E6">
-            <v>39.0169</v>
-          </cell>
-          <cell r="F6">
-            <v>5.5888</v>
-          </cell>
-          <cell r="G6">
-            <v>3.6522999999999999</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="D7">
-            <v>16</v>
-          </cell>
-          <cell r="E7">
-            <v>37.7652</v>
-          </cell>
-          <cell r="F7">
-            <v>0.91710000000000003</v>
-          </cell>
-          <cell r="G7">
-            <v>3.9735</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="D8">
-            <v>32</v>
-          </cell>
-          <cell r="E8">
-            <v>43.6539</v>
-          </cell>
-          <cell r="F8">
-            <v>0.1651</v>
-          </cell>
-          <cell r="G8">
-            <v>1.8986000000000001</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="E10">
-            <v>0</v>
-          </cell>
-          <cell r="F10">
-            <v>0.26300000000000001</v>
-          </cell>
-          <cell r="G10">
-            <v>0.19209999999999999</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="E11">
-            <v>0</v>
-          </cell>
-          <cell r="F11">
-            <v>0</v>
-          </cell>
-          <cell r="G11">
-            <v>0.13550000000000001</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="E12">
-            <v>28.887499999999999</v>
-          </cell>
-          <cell r="F12">
-            <v>11.911099999999999</v>
-          </cell>
-          <cell r="G12">
-            <v>7.1414999999999997</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="E13">
-            <v>24.7256</v>
-          </cell>
-          <cell r="F13">
-            <v>1.6279999999999999</v>
-          </cell>
-          <cell r="G13">
-            <v>12.668100000000001</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="E14">
-            <v>37.367199999999997</v>
-          </cell>
-          <cell r="F14">
-            <v>0.79590000000000005</v>
-          </cell>
-          <cell r="G14">
-            <v>2.649</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="E16">
-            <v>0</v>
-          </cell>
-          <cell r="F16">
-            <v>0</v>
-          </cell>
-          <cell r="G16">
-            <v>0.1724</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="E17">
-            <v>0</v>
-          </cell>
-          <cell r="F17">
-            <v>0.24340000000000001</v>
-          </cell>
-          <cell r="G17">
-            <v>0.26779999999999998</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="E18">
-            <v>8.0200999999999993</v>
-          </cell>
-          <cell r="F18">
-            <v>8.0200999999999993</v>
-          </cell>
-          <cell r="G18">
-            <v>14.3773</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="E19">
-            <v>3.4820000000000002</v>
-          </cell>
-          <cell r="F19">
-            <v>7.3723000000000001</v>
-          </cell>
-          <cell r="G19">
-            <v>12.925599999999999</v>
-          </cell>
-        </row>
-        <row r="20">
-          <cell r="E20">
-            <v>24.358799999999999</v>
-          </cell>
-          <cell r="F20">
-            <v>5.7351999999999999</v>
-          </cell>
-          <cell r="G20">
-            <v>2.1141000000000001</v>
-          </cell>
-        </row>
-        <row r="22">
-          <cell r="E22">
-            <v>0</v>
-          </cell>
-          <cell r="F22">
-            <v>0</v>
-          </cell>
-          <cell r="G22">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="23">
-          <cell r="E23">
-            <v>0</v>
-          </cell>
-          <cell r="F23">
-            <v>0.1153</v>
-          </cell>
-          <cell r="G23">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="24">
-          <cell r="E24">
-            <v>-2.86E-2</v>
-          </cell>
-          <cell r="F24">
-            <v>0.2611</v>
-          </cell>
-          <cell r="G24">
-            <v>0.21970000000000001</v>
-          </cell>
-        </row>
-        <row r="25">
-          <cell r="E25">
-            <v>-22.630199999999999</v>
-          </cell>
-          <cell r="F25">
-            <v>7.0137999999999998</v>
-          </cell>
-          <cell r="G25">
-            <v>46.412399999999998</v>
-          </cell>
-        </row>
-        <row r="26">
-          <cell r="E26">
-            <v>2.1263999999999998</v>
-          </cell>
-          <cell r="F26">
-            <v>2.6492</v>
-          </cell>
-          <cell r="G26">
-            <v>10.610300000000001</v>
-          </cell>
-        </row>
-        <row r="29">
-          <cell r="E29">
-            <v>-3.8346</v>
-          </cell>
-          <cell r="F29">
-            <v>0.52749999999999997</v>
-          </cell>
-          <cell r="G29">
-            <v>0.10730000000000001</v>
-          </cell>
-        </row>
-        <row r="30">
-          <cell r="E30">
-            <v>21.983799999999999</v>
-          </cell>
-          <cell r="F30">
-            <v>0</v>
-          </cell>
-          <cell r="G30">
-            <v>1.04E-2</v>
-          </cell>
-        </row>
-        <row r="31">
-          <cell r="E31">
-            <v>35.973199999999999</v>
-          </cell>
-          <cell r="F31">
-            <v>1.41E-2</v>
-          </cell>
-          <cell r="G31">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="32">
-          <cell r="E32">
-            <v>43.075600000000001</v>
-          </cell>
-          <cell r="F32">
-            <v>8.9700000000000002E-2</v>
-          </cell>
-          <cell r="G32">
-            <v>0.45300000000000001</v>
-          </cell>
-        </row>
-        <row r="33">
-          <cell r="E33">
-            <v>46.816899999999997</v>
-          </cell>
-          <cell r="F33">
-            <v>0.60450000000000004</v>
-          </cell>
-          <cell r="G33">
-            <v>0.50980000000000003</v>
-          </cell>
-        </row>
-        <row r="35">
-          <cell r="E35">
-            <v>0.3841</v>
-          </cell>
-          <cell r="F35">
-            <v>0.19589999999999999</v>
-          </cell>
-          <cell r="G35">
-            <v>7.7299999999999994E-2</v>
-          </cell>
-        </row>
-        <row r="36">
-          <cell r="E36">
-            <v>-5.0045000000000002</v>
-          </cell>
-          <cell r="F36">
-            <v>3.7900000000000003E-2</v>
-          </cell>
-          <cell r="G36">
-            <v>0.12720000000000001</v>
-          </cell>
-        </row>
-        <row r="37">
-          <cell r="E37">
-            <v>21.983799999999999</v>
-          </cell>
-          <cell r="F37">
-            <v>0.1396</v>
-          </cell>
-          <cell r="G37">
-            <v>0.1087</v>
-          </cell>
-        </row>
-        <row r="38">
-          <cell r="E38">
-            <v>35.933900000000001</v>
-          </cell>
-          <cell r="F38">
-            <v>0.15570000000000001</v>
-          </cell>
-          <cell r="G38">
-            <v>0.6431</v>
-          </cell>
-        </row>
-        <row r="39">
-          <cell r="E39">
-            <v>43.1629</v>
-          </cell>
-          <cell r="F39">
-            <v>0.13739999999999999</v>
-          </cell>
-          <cell r="G39">
-            <v>0.37040000000000001</v>
-          </cell>
-        </row>
-        <row r="41">
-          <cell r="E41">
-            <v>0</v>
-          </cell>
-          <cell r="F41">
-            <v>0</v>
-          </cell>
-          <cell r="G41">
-            <v>0.1724</v>
-          </cell>
-        </row>
-        <row r="42">
-          <cell r="E42">
-            <v>0.27200000000000002</v>
-          </cell>
-          <cell r="F42">
-            <v>2.86E-2</v>
-          </cell>
-          <cell r="G42">
-            <v>0.2636</v>
-          </cell>
-        </row>
-        <row r="43">
-          <cell r="E43">
-            <v>-5.7415000000000003</v>
-          </cell>
-          <cell r="F43">
-            <v>0.19089999999999999</v>
-          </cell>
-          <cell r="G43">
-            <v>0.74450000000000005</v>
-          </cell>
-        </row>
-        <row r="44">
-          <cell r="E44">
-            <v>21.6325</v>
-          </cell>
-          <cell r="F44">
-            <v>12.7317</v>
-          </cell>
-          <cell r="G44">
-            <v>2.7587999999999999</v>
-          </cell>
-        </row>
-        <row r="45">
-          <cell r="E45">
-            <v>36.095399999999998</v>
-          </cell>
-          <cell r="F45">
-            <v>0.41839999999999999</v>
-          </cell>
-          <cell r="G45">
-            <v>0.28089999999999998</v>
-          </cell>
-        </row>
-        <row r="47">
-          <cell r="E47">
-            <v>0</v>
-          </cell>
-          <cell r="F47">
-            <v>0</v>
-          </cell>
-          <cell r="G47">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="48">
-          <cell r="E48">
-            <v>0</v>
-          </cell>
-          <cell r="F48">
-            <v>0</v>
-          </cell>
-          <cell r="G48">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="49">
-          <cell r="E49">
-            <v>0.33560000000000001</v>
-          </cell>
-          <cell r="F49">
-            <v>9.2899999999999996E-2</v>
-          </cell>
-          <cell r="G49">
-            <v>0.40639999999999998</v>
-          </cell>
-        </row>
-        <row r="50">
-          <cell r="E50">
-            <v>-8.2013999999999996</v>
-          </cell>
-          <cell r="F50">
-            <v>42.866500000000002</v>
-          </cell>
-          <cell r="G50">
-            <v>5.8691000000000004</v>
-          </cell>
-        </row>
-        <row r="51">
-          <cell r="E51">
-            <v>21.259899999999998</v>
-          </cell>
-          <cell r="F51">
-            <v>9.0968999999999998</v>
-          </cell>
-          <cell r="G51">
-            <v>2.1303999999999998</v>
-          </cell>
-        </row>
-        <row r="54">
-          <cell r="E54">
-            <v>-3.8346</v>
-          </cell>
-          <cell r="F54">
-            <v>0.52749999999999997</v>
-          </cell>
-          <cell r="G54">
-            <v>0.10730000000000001</v>
-          </cell>
-        </row>
-        <row r="55">
-          <cell r="E55">
-            <v>39.221800000000002</v>
-          </cell>
-          <cell r="F55">
-            <v>0.83879999999999999</v>
-          </cell>
-          <cell r="G55">
-            <v>0.26179999999999998</v>
-          </cell>
-        </row>
-        <row r="56">
-          <cell r="E56">
-            <v>74.990200000000002</v>
-          </cell>
-          <cell r="F56">
-            <v>5.5888999999999998</v>
-          </cell>
-          <cell r="G56">
-            <v>3.3757999999999999</v>
-          </cell>
-        </row>
-        <row r="57">
-          <cell r="E57">
-            <v>80.340999999999994</v>
-          </cell>
-          <cell r="F57">
-            <v>2.9379</v>
-          </cell>
-          <cell r="G57">
-            <v>4.26</v>
-          </cell>
-        </row>
-        <row r="58">
-          <cell r="E58">
-            <v>90.113900000000001</v>
-          </cell>
-          <cell r="F58">
-            <v>1.6204000000000001</v>
-          </cell>
-          <cell r="G58">
-            <v>0.89080000000000004</v>
-          </cell>
-        </row>
-        <row r="60">
-          <cell r="E60">
-            <v>0.3841</v>
-          </cell>
-          <cell r="F60">
-            <v>0.19589999999999999</v>
-          </cell>
-          <cell r="G60">
-            <v>7.7299999999999994E-2</v>
-          </cell>
-        </row>
-        <row r="61">
-          <cell r="E61">
-            <v>-5.0045000000000002</v>
-          </cell>
-          <cell r="F61">
-            <v>3.7900000000000003E-2</v>
-          </cell>
-          <cell r="G61">
-            <v>0.12720000000000001</v>
-          </cell>
-        </row>
-        <row r="62">
-          <cell r="E62">
-            <v>50.832000000000001</v>
-          </cell>
-          <cell r="F62">
-            <v>11.8719</v>
-          </cell>
-          <cell r="G62">
-            <v>7.1719999999999997</v>
-          </cell>
-        </row>
-        <row r="63">
-          <cell r="E63">
-            <v>64.251800000000003</v>
-          </cell>
-          <cell r="F63">
-            <v>3.6684999999999999</v>
-          </cell>
-          <cell r="G63">
-            <v>5.6044</v>
-          </cell>
-        </row>
-        <row r="64">
-          <cell r="E64">
-            <v>80.218699999999998</v>
-          </cell>
-          <cell r="F64">
-            <v>3.2532000000000001</v>
-          </cell>
-          <cell r="G64">
-            <v>2.5999999999999999E-2</v>
-          </cell>
-        </row>
-        <row r="66">
-          <cell r="E66">
-            <v>0</v>
-          </cell>
-          <cell r="F66">
-            <v>0</v>
-          </cell>
-          <cell r="G66">
-            <v>0.1724</v>
-          </cell>
-        </row>
-        <row r="67">
-          <cell r="E67">
-            <v>0.27200000000000002</v>
-          </cell>
-          <cell r="F67">
-            <v>2.86E-2</v>
-          </cell>
-          <cell r="G67">
-            <v>0.2636</v>
-          </cell>
-        </row>
-        <row r="68">
-          <cell r="E68">
-            <v>2.2519</v>
-          </cell>
-          <cell r="F68">
-            <v>7.2564000000000002</v>
-          </cell>
-          <cell r="G68">
-            <v>14.3772</v>
-          </cell>
-        </row>
-        <row r="69">
-          <cell r="E69">
-            <v>24.073699999999999</v>
-          </cell>
-          <cell r="F69">
-            <v>4.8856000000000002</v>
-          </cell>
-          <cell r="G69">
-            <v>14.556699999999999</v>
-          </cell>
-        </row>
-        <row r="70">
-          <cell r="E70">
-            <v>61.642499999999998</v>
-          </cell>
-          <cell r="F70">
-            <v>2.1135999999999999</v>
-          </cell>
-          <cell r="G70">
-            <v>3.7351999999999999</v>
-          </cell>
-        </row>
-        <row r="72">
-          <cell r="E72">
-            <v>0</v>
-          </cell>
-          <cell r="F72">
-            <v>0</v>
-          </cell>
-          <cell r="G72">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="73">
-          <cell r="E73">
-            <v>0</v>
-          </cell>
-          <cell r="F73">
-            <v>0</v>
-          </cell>
-          <cell r="G73">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="74">
-          <cell r="E74">
-            <v>0.33560000000000001</v>
-          </cell>
-          <cell r="F74">
-            <v>9.2899999999999996E-2</v>
-          </cell>
-          <cell r="G74">
-            <v>0.40639999999999998</v>
-          </cell>
-        </row>
-        <row r="75">
-          <cell r="E75">
-            <v>-15.534700000000001</v>
-          </cell>
-          <cell r="F75">
-            <v>21.0212</v>
-          </cell>
-          <cell r="G75">
-            <v>45.945999999999998</v>
-          </cell>
-        </row>
-        <row r="76">
-          <cell r="E76">
-            <v>21.519100000000002</v>
-          </cell>
-          <cell r="F76">
-            <v>11.7506</v>
-          </cell>
-          <cell r="G76">
-            <v>3.4872999999999998</v>
-          </cell>
-        </row>
-        <row r="79">
-          <cell r="E79">
-            <v>0</v>
-          </cell>
-          <cell r="F79">
-            <v>0</v>
-          </cell>
-          <cell r="G79">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="80">
-          <cell r="E80">
-            <v>22.095500000000001</v>
-          </cell>
-          <cell r="F80">
-            <v>1.0859000000000001</v>
-          </cell>
-          <cell r="G80">
-            <v>0.33550000000000002</v>
-          </cell>
-        </row>
-        <row r="81">
-          <cell r="E81">
-            <v>60.938499999999998</v>
-          </cell>
-          <cell r="F81">
-            <v>8.7289999999999992</v>
-          </cell>
-          <cell r="G81">
-            <v>5.2798999999999996</v>
-          </cell>
-        </row>
-        <row r="82">
-          <cell r="E82">
-            <v>65.484899999999996</v>
-          </cell>
-          <cell r="F82">
-            <v>5.2960000000000003</v>
-          </cell>
-          <cell r="G82">
-            <v>7.3456999999999999</v>
-          </cell>
-        </row>
-        <row r="83">
-          <cell r="E83">
-            <v>81.555199999999999</v>
-          </cell>
-          <cell r="F83">
-            <v>3.2852000000000001</v>
-          </cell>
-          <cell r="G83">
-            <v>1.3673</v>
-          </cell>
-        </row>
-        <row r="85">
-          <cell r="E85">
-            <v>0</v>
-          </cell>
-          <cell r="F85">
-            <v>0</v>
-          </cell>
-          <cell r="G85">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="86">
-          <cell r="E86">
-            <v>0</v>
-          </cell>
-          <cell r="F86">
-            <v>0</v>
-          </cell>
-          <cell r="G86">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="87">
-          <cell r="E87">
-            <v>36.889200000000002</v>
-          </cell>
-          <cell r="F87">
-            <v>15.129200000000001</v>
-          </cell>
-          <cell r="G87">
-            <v>9.2810000000000006</v>
-          </cell>
-        </row>
-        <row r="88">
-          <cell r="E88">
-            <v>44.071300000000001</v>
-          </cell>
-          <cell r="F88">
-            <v>6.0250000000000004</v>
-          </cell>
-          <cell r="G88">
-            <v>8.9834999999999994</v>
-          </cell>
-        </row>
-        <row r="89">
-          <cell r="E89">
-            <v>64.968299999999999</v>
-          </cell>
-          <cell r="F89">
-            <v>5.4389000000000003</v>
-          </cell>
-          <cell r="G89">
-            <v>0.2442</v>
-          </cell>
-        </row>
-        <row r="91">
-          <cell r="E91">
-            <v>0</v>
-          </cell>
-          <cell r="F91">
-            <v>0</v>
-          </cell>
-          <cell r="G91">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="92">
-          <cell r="E92">
-            <v>0</v>
-          </cell>
-          <cell r="F92">
-            <v>0</v>
-          </cell>
-          <cell r="G92">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="93">
-          <cell r="E93">
-            <v>7.5978000000000003</v>
-          </cell>
-          <cell r="F93">
-            <v>7.5978000000000003</v>
-          </cell>
-          <cell r="G93">
-            <v>13.578099999999999</v>
-          </cell>
-        </row>
-        <row r="94">
-          <cell r="E94">
-            <v>4.1816000000000004</v>
-          </cell>
-          <cell r="F94">
-            <v>7.3007</v>
-          </cell>
-          <cell r="G94">
-            <v>19.327999999999999</v>
-          </cell>
-        </row>
-        <row r="95">
-          <cell r="E95">
-            <v>39.947899999999997</v>
-          </cell>
-          <cell r="F95">
-            <v>2.8664000000000001</v>
-          </cell>
-          <cell r="G95">
-            <v>5.8739999999999997</v>
-          </cell>
-        </row>
-        <row r="97">
-          <cell r="E97">
-            <v>0</v>
-          </cell>
-          <cell r="F97">
-            <v>0</v>
-          </cell>
-          <cell r="G97">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="98">
-          <cell r="E98">
-            <v>0</v>
-          </cell>
-          <cell r="F98">
-            <v>0</v>
-          </cell>
-          <cell r="G98">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="99">
-          <cell r="E99">
-            <v>0</v>
-          </cell>
-          <cell r="F99">
-            <v>0</v>
-          </cell>
-          <cell r="G99">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="100">
-          <cell r="E100">
-            <v>13.1912</v>
-          </cell>
-          <cell r="F100">
-            <v>43.831099999999999</v>
-          </cell>
-          <cell r="G100">
-            <v>18.806100000000001</v>
-          </cell>
-        </row>
-        <row r="101">
-          <cell r="E101">
-            <v>-1.0195000000000001</v>
-          </cell>
-          <cell r="F101">
-            <v>10.539300000000001</v>
-          </cell>
-          <cell r="G101">
-            <v>15.641400000000001</v>
-          </cell>
-        </row>
-      </sheetData>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -7786,7 +6868,7 @@
   <dimension ref="A1:G101"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection sqref="A1:G101"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7853,10 +6935,10 @@
         <v>0</v>
       </c>
       <c r="F4">
-        <v>3.9249999999999998</v>
+        <v>7.5114000000000001</v>
       </c>
       <c r="G4">
-        <v>4.0259</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -7873,13 +6955,13 @@
         <v>4</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>-4.2131999999999996</v>
       </c>
       <c r="F5">
-        <v>10.418100000000001</v>
+        <v>0.86280000000000001</v>
       </c>
       <c r="G5">
-        <v>6.7363999999999997</v>
+        <v>17.860399999999998</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -7896,13 +6978,13 @@
         <v>8</v>
       </c>
       <c r="E6">
-        <v>6.5096999999999996</v>
+        <v>1.7411000000000001</v>
       </c>
       <c r="F6">
-        <v>12.7606</v>
+        <v>1.2144999999999999</v>
       </c>
       <c r="G6">
-        <v>3.0034999999999998</v>
+        <v>8.0541</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -7919,13 +7001,13 @@
         <v>16</v>
       </c>
       <c r="E7">
-        <v>5.2363999999999997</v>
+        <v>2.5525000000000002</v>
       </c>
       <c r="F7">
-        <v>8.9398</v>
+        <v>9.5643999999999991</v>
       </c>
       <c r="G7">
-        <v>0.93010000000000004</v>
+        <v>11.3103</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -7942,13 +7024,13 @@
         <v>32</v>
       </c>
       <c r="E8">
-        <v>1.3164</v>
+        <v>0.10730000000000001</v>
       </c>
       <c r="F8">
-        <v>3.5476000000000001</v>
+        <v>4.4924999999999997</v>
       </c>
       <c r="G8">
-        <v>1.8855</v>
+        <v>4.9554999999999998</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -7965,13 +7047,13 @@
         <v>2</v>
       </c>
       <c r="E10">
-        <v>-4.1947000000000001</v>
+        <v>0</v>
       </c>
       <c r="F10">
-        <v>4.2954999999999997</v>
+        <v>2.1156000000000001</v>
       </c>
       <c r="G10">
-        <v>4.1947000000000001</v>
+        <v>4.3742999999999999</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -7991,10 +7073,10 @@
         <v>0</v>
       </c>
       <c r="F11">
-        <v>17.940000000000001</v>
+        <v>12.2658</v>
       </c>
       <c r="G11">
-        <v>14.984999999999999</v>
+        <v>10.8072</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
@@ -8011,13 +7093,13 @@
         <v>8</v>
       </c>
       <c r="E12">
-        <v>14.7575</v>
+        <v>11.5968</v>
       </c>
       <c r="F12">
-        <v>2.6738</v>
+        <v>11.7957</v>
       </c>
       <c r="G12">
-        <v>3.7103999999999999</v>
+        <v>4.2348999999999997</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
@@ -8034,13 +7116,13 @@
         <v>16</v>
       </c>
       <c r="E13">
-        <v>8.1292000000000009</v>
+        <v>6.9654999999999996</v>
       </c>
       <c r="F13">
-        <v>6.3948</v>
+        <v>7.2824999999999998</v>
       </c>
       <c r="G13">
-        <v>1.7636000000000001</v>
+        <v>9.5877999999999997</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
@@ -8057,13 +7139,13 @@
         <v>32</v>
       </c>
       <c r="E14">
-        <v>17.009599999999999</v>
+        <v>11.9672</v>
       </c>
       <c r="F14">
-        <v>10.0563</v>
+        <v>6.2652999999999999</v>
       </c>
       <c r="G14">
-        <v>5.4840999999999998</v>
+        <v>6.0743999999999998</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
@@ -8080,13 +7162,13 @@
         <v>2</v>
       </c>
       <c r="E16">
-        <v>0</v>
+        <v>0.89839999999999998</v>
       </c>
       <c r="F16">
-        <v>0</v>
+        <v>1.9399</v>
       </c>
       <c r="G16">
-        <v>0</v>
+        <v>1.4380999999999999</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
@@ -8103,13 +7185,13 @@
         <v>4</v>
       </c>
       <c r="E17">
-        <v>0</v>
+        <v>2.33</v>
       </c>
       <c r="F17">
-        <v>15.151</v>
+        <v>6.1346999999999996</v>
       </c>
       <c r="G17">
-        <v>2.0036999999999998</v>
+        <v>2.6269999999999998</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
@@ -8126,13 +7208,13 @@
         <v>8</v>
       </c>
       <c r="E18">
-        <v>9.5718999999999994</v>
+        <v>9.4778000000000002</v>
       </c>
       <c r="F18">
-        <v>9.1227</v>
+        <v>5.2954999999999997</v>
       </c>
       <c r="G18">
-        <v>4.6401000000000003</v>
+        <v>2.9828999999999999</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
@@ -8149,13 +7231,13 @@
         <v>16</v>
       </c>
       <c r="E19">
-        <v>-2.4571999999999998</v>
+        <v>2.3946999999999998</v>
       </c>
       <c r="F19">
-        <v>15.920199999999999</v>
+        <v>22.511700000000001</v>
       </c>
       <c r="G19">
-        <v>30.564800000000002</v>
+        <v>19.389800000000001</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
@@ -8172,13 +7254,13 @@
         <v>32</v>
       </c>
       <c r="E20">
-        <v>12.7744</v>
+        <v>10.9771</v>
       </c>
       <c r="F20">
-        <v>0.97250000000000003</v>
+        <v>2.9529999999999998</v>
       </c>
       <c r="G20">
-        <v>3.3437999999999999</v>
+        <v>6.7450999999999999</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
@@ -8198,10 +7280,10 @@
         <v>0</v>
       </c>
       <c r="F22">
-        <v>0</v>
+        <v>0.52290000000000003</v>
       </c>
       <c r="G22">
-        <v>0</v>
+        <v>1.0544</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
@@ -8218,13 +7300,13 @@
         <v>4</v>
       </c>
       <c r="E23">
-        <v>0</v>
+        <v>0.66269999999999996</v>
       </c>
       <c r="F23">
-        <v>2.5548999999999999</v>
+        <v>1.9568000000000001</v>
       </c>
       <c r="G23">
-        <v>0.54090000000000005</v>
+        <v>0.6724</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
@@ -8244,10 +7326,10 @@
         <v>0</v>
       </c>
       <c r="F24">
-        <v>24.306999999999999</v>
+        <v>4.7347000000000001</v>
       </c>
       <c r="G24">
-        <v>3.9908999999999999</v>
+        <v>2.5838999999999999</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
@@ -8264,13 +7346,13 @@
         <v>16</v>
       </c>
       <c r="E25">
-        <v>11.161300000000001</v>
+        <v>6.9943</v>
       </c>
       <c r="F25">
-        <v>52.145499999999998</v>
+        <v>32.706200000000003</v>
       </c>
       <c r="G25">
-        <v>25.402899999999999</v>
+        <v>13.144600000000001</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
@@ -8287,13 +7369,13 @@
         <v>32</v>
       </c>
       <c r="E26">
-        <v>1.4196</v>
+        <v>-0.38519999999999999</v>
       </c>
       <c r="F26">
-        <v>7.9821</v>
+        <v>12.5223</v>
       </c>
       <c r="G26">
-        <v>2.2231000000000001</v>
+        <v>5.5522</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
@@ -8318,13 +7400,13 @@
         <v>2</v>
       </c>
       <c r="E29">
-        <v>-3.7273000000000001</v>
+        <v>14.138400000000001</v>
       </c>
       <c r="F29">
-        <v>0.19769999999999999</v>
+        <v>9.8666</v>
       </c>
       <c r="G29">
-        <v>3.7273000000000001</v>
+        <v>1.6604000000000001</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
@@ -8341,13 +7423,13 @@
         <v>4</v>
       </c>
       <c r="E30">
-        <v>-3.8555000000000001</v>
+        <v>6.1501000000000001</v>
       </c>
       <c r="F30">
-        <v>1.21E-2</v>
+        <v>0.82879999999999998</v>
       </c>
       <c r="G30">
-        <v>5.1142000000000003</v>
+        <v>14.8104</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
@@ -8364,13 +7446,13 @@
         <v>8</v>
       </c>
       <c r="E31">
-        <v>-2.2559</v>
+        <v>2.9178000000000002</v>
       </c>
       <c r="F31">
-        <v>7.1000000000000004E-3</v>
+        <v>1.8715999999999999</v>
       </c>
       <c r="G31">
-        <v>0.78759999999999997</v>
+        <v>7.3989000000000003</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
@@ -8387,13 +7469,13 @@
         <v>16</v>
       </c>
       <c r="E32">
-        <v>-0.38490000000000002</v>
+        <v>4.1162000000000001</v>
       </c>
       <c r="F32">
-        <v>1.0134000000000001</v>
+        <v>0.9607</v>
       </c>
       <c r="G32">
-        <v>1.3626</v>
+        <v>12.389699999999999</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
@@ -8410,13 +7492,13 @@
         <v>32</v>
       </c>
       <c r="E33">
-        <v>-0.12189999999999999</v>
+        <v>3.3426999999999998</v>
       </c>
       <c r="F33">
-        <v>1.3399000000000001</v>
+        <v>1.9303999999999999</v>
       </c>
       <c r="G33">
-        <v>4.4123999999999999</v>
+        <v>6.1835000000000004</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
@@ -8433,13 +7515,13 @@
         <v>2</v>
       </c>
       <c r="E35">
-        <v>-4.758</v>
+        <v>2.1198000000000001</v>
       </c>
       <c r="F35">
-        <v>3.7322000000000002</v>
+        <v>2.1198000000000001</v>
       </c>
       <c r="G35">
-        <v>4.758</v>
+        <v>5.4871999999999996</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
@@ -8456,13 +7538,13 @@
         <v>4</v>
       </c>
       <c r="E36">
-        <v>-5.0195999999999996</v>
+        <v>19.444400000000002</v>
       </c>
       <c r="F36">
-        <v>6.7953999999999999</v>
+        <v>9.6945999999999994</v>
       </c>
       <c r="G36">
-        <v>5.0195999999999996</v>
+        <v>0.23780000000000001</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
@@ -8479,13 +7561,13 @@
         <v>8</v>
       </c>
       <c r="E37">
-        <v>0.56699999999999995</v>
+        <v>18.007400000000001</v>
       </c>
       <c r="F37">
-        <v>4.1631999999999998</v>
+        <v>5.0204000000000004</v>
       </c>
       <c r="G37">
-        <v>5.4642999999999997</v>
+        <v>4.6916000000000002</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
@@ -8502,13 +7584,13 @@
         <v>16</v>
       </c>
       <c r="E38">
-        <v>6.7910000000000004</v>
+        <v>20.5471</v>
       </c>
       <c r="F38">
-        <v>1.742</v>
+        <v>3.8872</v>
       </c>
       <c r="G38">
-        <v>3.8494000000000002</v>
+        <v>4.1142000000000003</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
@@ -8525,13 +7607,13 @@
         <v>32</v>
       </c>
       <c r="E39">
-        <v>14.6713</v>
+        <v>19.296500000000002</v>
       </c>
       <c r="F39">
-        <v>1.5539000000000001</v>
+        <v>2.6673</v>
       </c>
       <c r="G39">
-        <v>3.3325999999999998</v>
+        <v>3.7086999999999999</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
@@ -8548,13 +7630,13 @@
         <v>2</v>
       </c>
       <c r="E41">
-        <v>0</v>
+        <v>2.1198000000000001</v>
       </c>
       <c r="F41">
-        <v>0</v>
+        <v>0.105</v>
       </c>
       <c r="G41">
-        <v>0</v>
+        <v>1.8287</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
@@ -8571,13 +7653,13 @@
         <v>4</v>
       </c>
       <c r="E42">
-        <v>0</v>
+        <v>8.7388999999999992</v>
       </c>
       <c r="F42">
-        <v>25.215699999999998</v>
+        <v>4.7906000000000004</v>
       </c>
       <c r="G42">
-        <v>0</v>
+        <v>2.1029</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
@@ -8594,13 +7676,13 @@
         <v>8</v>
       </c>
       <c r="E43">
-        <v>-14.002599999999999</v>
+        <v>18.037700000000001</v>
       </c>
       <c r="F43">
-        <v>5.3918999999999997</v>
+        <v>4.5000999999999998</v>
       </c>
       <c r="G43">
-        <v>19.160699999999999</v>
+        <v>4.8689999999999998</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
@@ -8617,13 +7699,13 @@
         <v>16</v>
       </c>
       <c r="E44">
-        <v>6.6069000000000004</v>
+        <v>28.906600000000001</v>
       </c>
       <c r="F44">
-        <v>3.9988999999999999</v>
+        <v>6.1161000000000003</v>
       </c>
       <c r="G44">
-        <v>10.2113</v>
+        <v>4.7591000000000001</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
@@ -8640,13 +7722,13 @@
         <v>32</v>
       </c>
       <c r="E45">
-        <v>19.349699999999999</v>
+        <v>28.3504</v>
       </c>
       <c r="F45">
-        <v>2.1896</v>
+        <v>2.3285</v>
       </c>
       <c r="G45">
-        <v>2.4683000000000002</v>
+        <v>2.1880000000000002</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
@@ -8663,13 +7745,13 @@
         <v>2</v>
       </c>
       <c r="E47">
-        <v>0</v>
+        <v>2.5194000000000001</v>
       </c>
       <c r="F47">
-        <v>0</v>
+        <v>0.95069999999999999</v>
       </c>
       <c r="G47">
-        <v>0</v>
+        <v>0.64390000000000003</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
@@ -8686,13 +7768,13 @@
         <v>4</v>
       </c>
       <c r="E48">
-        <v>0</v>
+        <v>4.6391</v>
       </c>
       <c r="F48">
-        <v>0</v>
+        <v>0.6764</v>
       </c>
       <c r="G48">
-        <v>0.54090000000000005</v>
+        <v>0.52300000000000002</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
@@ -8709,13 +7791,13 @@
         <v>8</v>
       </c>
       <c r="E49">
-        <v>2.4843000000000002</v>
+        <v>7.8101000000000003</v>
       </c>
       <c r="F49">
-        <v>23.7074</v>
+        <v>3.1709999999999998</v>
       </c>
       <c r="G49">
-        <v>1.1013999999999999</v>
+        <v>8.3347999999999995</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
@@ -8732,13 +7814,13 @@
         <v>16</v>
       </c>
       <c r="E50">
-        <v>4.8021000000000003</v>
+        <v>17.975300000000001</v>
       </c>
       <c r="F50">
-        <v>72.534099999999995</v>
+        <v>26.922499999999999</v>
       </c>
       <c r="G50">
-        <v>16.4925</v>
+        <v>18.184000000000001</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
@@ -8755,13 +7837,13 @@
         <v>32</v>
       </c>
       <c r="E51">
-        <v>19.631599999999999</v>
+        <v>33.553199999999997</v>
       </c>
       <c r="F51">
-        <v>9.6737000000000002</v>
+        <v>5.0507999999999997</v>
       </c>
       <c r="G51">
-        <v>4.0586000000000002</v>
+        <v>1.6419999999999999</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.2">
@@ -8786,13 +7868,13 @@
         <v>2</v>
       </c>
       <c r="E54">
-        <v>-3.7273000000000001</v>
+        <v>14.138400000000001</v>
       </c>
       <c r="F54">
-        <v>0.19769999999999999</v>
+        <v>9.8666</v>
       </c>
       <c r="G54">
-        <v>3.7273000000000001</v>
+        <v>1.6604000000000001</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.2">
@@ -8809,13 +7891,13 @@
         <v>4</v>
       </c>
       <c r="E55">
-        <v>19.430900000000001</v>
+        <v>27.176400000000001</v>
       </c>
       <c r="F55">
-        <v>1.1519999999999999</v>
+        <v>0.83860000000000001</v>
       </c>
       <c r="G55">
-        <v>3.9763999999999999</v>
+        <v>12.265000000000001</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.2">
@@ -8832,13 +7914,13 @@
         <v>8</v>
       </c>
       <c r="E56">
-        <v>60.057299999999998</v>
+        <v>64.941400000000002</v>
       </c>
       <c r="F56">
-        <v>8.9292999999999996</v>
+        <v>9.8327000000000009</v>
       </c>
       <c r="G56">
-        <v>5.6719999999999997</v>
+        <v>3.7345999999999999</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.2">
@@ -8855,13 +7937,13 @@
         <v>16</v>
       </c>
       <c r="E57">
-        <v>65.639899999999997</v>
+        <v>71.692099999999996</v>
       </c>
       <c r="F57">
-        <v>1.7971999999999999</v>
+        <v>4.3781999999999996</v>
       </c>
       <c r="G57">
-        <v>9.4620999999999995</v>
+        <v>6.4366000000000003</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.2">
@@ -8878,13 +7960,13 @@
         <v>32</v>
       </c>
       <c r="E58">
-        <v>82.009</v>
+        <v>82.616200000000006</v>
       </c>
       <c r="F58">
-        <v>1.1005</v>
+        <v>1.7383999999999999</v>
       </c>
       <c r="G58">
-        <v>2.3216000000000001</v>
+        <v>1.6465000000000001</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.2">
@@ -8901,13 +7983,13 @@
         <v>2</v>
       </c>
       <c r="E60">
-        <v>-4.758</v>
+        <v>2.1198000000000001</v>
       </c>
       <c r="F60">
-        <v>3.7322000000000002</v>
+        <v>2.1198000000000001</v>
       </c>
       <c r="G60">
-        <v>4.758</v>
+        <v>5.4871999999999996</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.2">
@@ -8924,13 +8006,13 @@
         <v>4</v>
       </c>
       <c r="E61">
-        <v>-5.0195999999999996</v>
+        <v>19.444400000000002</v>
       </c>
       <c r="F61">
-        <v>6.7953999999999999</v>
+        <v>9.6945999999999994</v>
       </c>
       <c r="G61">
-        <v>5.0195999999999996</v>
+        <v>0.23780000000000001</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.2">
@@ -8947,13 +8029,13 @@
         <v>8</v>
       </c>
       <c r="E62">
-        <v>34.736400000000003</v>
+        <v>50.0047</v>
       </c>
       <c r="F62">
-        <v>8.2575000000000003</v>
+        <v>9.8545999999999996</v>
       </c>
       <c r="G62">
-        <v>11.739000000000001</v>
+        <v>5.5377000000000001</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.2">
@@ -8970,13 +8052,13 @@
         <v>16</v>
       </c>
       <c r="E63">
-        <v>47.8063</v>
+        <v>54.768300000000004</v>
       </c>
       <c r="F63">
-        <v>7.4078999999999997</v>
+        <v>5.3022</v>
       </c>
       <c r="G63">
-        <v>7.7244999999999999</v>
+        <v>8.3107000000000006</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.2">
@@ -8993,13 +8075,13 @@
         <v>32</v>
       </c>
       <c r="E64">
-        <v>71.803899999999999</v>
+        <v>73.442099999999996</v>
       </c>
       <c r="F64">
-        <v>1.0665</v>
+        <v>1.6975</v>
       </c>
       <c r="G64">
-        <v>4.6390000000000002</v>
+        <v>2.6516000000000002</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.2">
@@ -9016,13 +8098,13 @@
         <v>2</v>
       </c>
       <c r="E66">
-        <v>0</v>
+        <v>2.1198000000000001</v>
       </c>
       <c r="F66">
-        <v>0</v>
+        <v>0.105</v>
       </c>
       <c r="G66">
-        <v>0</v>
+        <v>1.8287</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.2">
@@ -9039,13 +8121,13 @@
         <v>4</v>
       </c>
       <c r="E67">
-        <v>0</v>
+        <v>8.7388999999999992</v>
       </c>
       <c r="F67">
-        <v>25.215699999999998</v>
+        <v>4.7906000000000004</v>
       </c>
       <c r="G67">
-        <v>0</v>
+        <v>2.1029</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.2">
@@ -9062,13 +8144,13 @@
         <v>8</v>
       </c>
       <c r="E68">
-        <v>0.72270000000000001</v>
+        <v>24.0578</v>
       </c>
       <c r="F68">
-        <v>6.9939</v>
+        <v>3.6305000000000001</v>
       </c>
       <c r="G68">
-        <v>9.2979000000000003</v>
+        <v>12.427899999999999</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.2">
@@ -9085,13 +8167,13 @@
         <v>16</v>
       </c>
       <c r="E69">
-        <v>7.9356999999999998</v>
+        <v>29.044499999999999</v>
       </c>
       <c r="F69">
-        <v>7.6985999999999999</v>
+        <v>3.8285999999999998</v>
       </c>
       <c r="G69">
-        <v>18.066199999999998</v>
+        <v>4.5978000000000003</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.2">
@@ -9108,13 +8190,13 @@
         <v>32</v>
       </c>
       <c r="E70">
-        <v>50.1355</v>
+        <v>56.591500000000003</v>
       </c>
       <c r="F70">
-        <v>6.8491999999999997</v>
+        <v>7.9172000000000002</v>
       </c>
       <c r="G70">
-        <v>11.669600000000001</v>
+        <v>9.2364999999999995</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.2">
@@ -9131,13 +8213,13 @@
         <v>2</v>
       </c>
       <c r="E72">
-        <v>0</v>
+        <v>2.5194000000000001</v>
       </c>
       <c r="F72">
-        <v>0</v>
+        <v>0.95069999999999999</v>
       </c>
       <c r="G72">
-        <v>0</v>
+        <v>0.64390000000000003</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.2">
@@ -9154,13 +8236,13 @@
         <v>4</v>
       </c>
       <c r="E73">
-        <v>0</v>
+        <v>4.6391</v>
       </c>
       <c r="F73">
-        <v>0</v>
+        <v>0.6764</v>
       </c>
       <c r="G73">
-        <v>0.54090000000000005</v>
+        <v>0.52300000000000002</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.2">
@@ -9177,13 +8259,13 @@
         <v>8</v>
       </c>
       <c r="E74">
-        <v>2.4843000000000002</v>
+        <v>7.8101000000000003</v>
       </c>
       <c r="F74">
-        <v>23.7074</v>
+        <v>3.1709999999999998</v>
       </c>
       <c r="G74">
-        <v>1.1013999999999999</v>
+        <v>8.3347999999999995</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.2">
@@ -9200,13 +8282,13 @@
         <v>16</v>
       </c>
       <c r="E75">
-        <v>5.3387000000000002</v>
+        <v>14.9391</v>
       </c>
       <c r="F75">
-        <v>69.257300000000001</v>
+        <v>39.0229</v>
       </c>
       <c r="G75">
-        <v>16.068899999999999</v>
+        <v>8.0741999999999994</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.2">
@@ -9223,13 +8305,13 @@
         <v>32</v>
       </c>
       <c r="E76">
-        <v>16.480899999999998</v>
+        <v>31.3813</v>
       </c>
       <c r="F76">
-        <v>8.6862999999999992</v>
+        <v>7.8407999999999998</v>
       </c>
       <c r="G76">
-        <v>5.1459999999999999</v>
+        <v>5.3498000000000001</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.2">
@@ -9274,13 +8356,13 @@
         <v>4</v>
       </c>
       <c r="E80">
-        <v>22.095500000000001</v>
+        <v>23.041</v>
       </c>
       <c r="F80">
-        <v>0.78269999999999995</v>
+        <v>1.1405000000000001</v>
       </c>
       <c r="G80">
-        <v>0.33550000000000002</v>
+        <v>0.34989999999999999</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.2">
@@ -9297,13 +8379,13 @@
         <v>8</v>
       </c>
       <c r="E81">
-        <v>60.938499999999998</v>
+        <v>62.512300000000003</v>
       </c>
       <c r="F81">
-        <v>8.7289999999999992</v>
+        <v>8.9603999999999999</v>
       </c>
       <c r="G81">
-        <v>5.2868000000000004</v>
+        <v>5.8324999999999996</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.2">
@@ -9320,13 +8402,13 @@
         <v>16</v>
       </c>
       <c r="E82">
-        <v>65.623999999999995</v>
+        <v>69.859300000000005</v>
       </c>
       <c r="F82">
-        <v>1.2827</v>
+        <v>3.6105</v>
       </c>
       <c r="G82">
-        <v>9.7922999999999991</v>
+        <v>4.1814999999999998</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.2">
@@ -9343,13 +8425,13 @@
         <v>32</v>
       </c>
       <c r="E83">
-        <v>81.912199999999999</v>
+        <v>81.811800000000005</v>
       </c>
       <c r="F83">
-        <v>0.92810000000000004</v>
+        <v>2.9474999999999998</v>
       </c>
       <c r="G83">
-        <v>2.0956000000000001</v>
+        <v>2.0724999999999998</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.2">
@@ -9412,13 +8494,13 @@
         <v>8</v>
       </c>
       <c r="E87">
-        <v>37.001899999999999</v>
+        <v>38.472299999999997</v>
       </c>
       <c r="F87">
-        <v>15.241899999999999</v>
+        <v>15.790100000000001</v>
       </c>
       <c r="G87">
-        <v>9.1683000000000003</v>
+        <v>9.6852999999999998</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.2">
@@ -9435,13 +8517,13 @@
         <v>16</v>
       </c>
       <c r="E88">
-        <v>41.823599999999999</v>
+        <v>42.733499999999999</v>
       </c>
       <c r="F88">
-        <v>4.7426000000000004</v>
+        <v>5.2157999999999998</v>
       </c>
       <c r="G88">
-        <v>10.4673</v>
+        <v>10.7974</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.2">
@@ -9458,13 +8540,13 @@
         <v>32</v>
       </c>
       <c r="E89">
-        <v>66.936499999999995</v>
+        <v>67.298500000000004</v>
       </c>
       <c r="F89">
-        <v>2.1894</v>
+        <v>2.0657999999999999</v>
       </c>
       <c r="G89">
-        <v>5.5594999999999999</v>
+        <v>3.0792000000000002</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.2">
@@ -9527,13 +8609,13 @@
         <v>8</v>
       </c>
       <c r="E93">
-        <v>7.7187000000000001</v>
+        <v>8.1956000000000007</v>
       </c>
       <c r="F93">
-        <v>7.7187000000000001</v>
+        <v>8.1956000000000007</v>
       </c>
       <c r="G93">
-        <v>13.3538</v>
+        <v>14.3345</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.2">
@@ -9550,13 +8632,13 @@
         <v>16</v>
       </c>
       <c r="E94">
-        <v>1.585</v>
+        <v>-0.11559999999999999</v>
       </c>
       <c r="F94">
-        <v>4.4302999999999999</v>
+        <v>0.89100000000000001</v>
       </c>
       <c r="G94">
-        <v>9.4555000000000007</v>
+        <v>5.3121999999999998</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.2">
@@ -9573,13 +8655,13 @@
         <v>32</v>
       </c>
       <c r="E95">
-        <v>38.2896</v>
+        <v>39.099899999999998</v>
       </c>
       <c r="F95">
-        <v>9.0564</v>
+        <v>10.3355</v>
       </c>
       <c r="G95">
-        <v>13.071199999999999</v>
+        <v>13.2272</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.2">
@@ -9665,13 +8747,13 @@
         <v>16</v>
       </c>
       <c r="E100">
-        <v>0.56359999999999999</v>
+        <v>-13.893599999999999</v>
       </c>
       <c r="F100">
-        <v>13.351699999999999</v>
+        <v>16.775700000000001</v>
       </c>
       <c r="G100">
-        <v>19.9679</v>
+        <v>20.035699999999999</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.2">
@@ -9688,13 +8770,13 @@
         <v>32</v>
       </c>
       <c r="E101">
-        <v>-2.7039</v>
+        <v>-1.4442999999999999</v>
       </c>
       <c r="F101">
-        <v>12.7332</v>
+        <v>15.6097</v>
       </c>
       <c r="G101">
-        <v>4.8808999999999996</v>
+        <v>12.385899999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>